<commit_message>
chang excel then builded
</commit_message>
<xml_diff>
--- a/public/importTenTen.xlsx
+++ b/public/importTenTen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ManhLe\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Projects\JAPAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06CD2DE-DDF9-4112-BAD8-D1E66B65E8C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367C8E75-6DF8-4BC4-8163-61C1C7782962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{08C9228A-C622-427E-A321-C7580DF990E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="11160" xr2:uid="{08C9228A-C622-427E-A321-C7580DF990E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>業種</t>
   </si>
@@ -72,27 +72,18 @@
     <t>黒木美紀</t>
   </si>
   <si>
-    <t>Doãn Trí Bình</t>
-  </si>
-  <si>
     <t>binhdt@vlx.com</t>
   </si>
   <si>
     <t>Sky.com</t>
   </si>
   <si>
-    <t>lon.com</t>
-  </si>
-  <si>
     <t>hay.com</t>
   </si>
   <si>
     <t>gamenet.com</t>
   </si>
   <si>
-    <t>lch.com</t>
-  </si>
-  <si>
     <t>ToshoYoam</t>
   </si>
   <si>
@@ -151,6 +142,18 @@
   </si>
   <si>
     <t>binhhoam@gmail.com</t>
+  </si>
+  <si>
+    <t>SAM SAM</t>
+  </si>
+  <si>
+    <t>skybabies.com</t>
+  </si>
+  <si>
+    <t>lichntb.com</t>
+  </si>
+  <si>
+    <t>郵便番号</t>
   </si>
 </sst>
 </file>
@@ -558,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6278D670-84B2-4E62-9218-249CA754B788}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD37"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,9 +576,10 @@
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="24.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,13 +601,16 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -612,105 +619,120 @@
         <v>9</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="H2">
+        <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="H3">
+        <v>10000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="H4">
+        <v>10000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="H5">
+        <v>10000</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="H6">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>